<commit_message>
#63 Fixed ToMapOptionProcessor to properly handle ignoreXxxx options. Also refactored Options class to be able to link Options between parent.
</commit_message>
<xml_diff>
--- a/example/optionExample.xlsx
+++ b/example/optionExample.xlsx
@@ -1,32 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9D05D5-4175-4F93-AC30-B8A968ADA289}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11230" activeTab="2" xr2:uid="{63327964-0F50-4074-8F85-858A1CE1D5F7}"/>
+    <workbookView xWindow="1380" yWindow="-108" windowWidth="29448" windowHeight="17496" activeTab="1" xr2:uid="{63327964-0F50-4074-8F85-858A1CE1D5F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="cellTypes" sheetId="1" r:id="rId1"/>
+    <sheet name="readAs" sheetId="2" r:id="rId2"/>
+    <sheet name="limit" sheetId="3" r:id="rId3"/>
+    <sheet name="toMap" sheetId="9" r:id="rId4"/>
+    <sheet name="fieldType" sheetId="10" r:id="rId5"/>
+    <sheet name="syntaxSugar" sheetId="11" r:id="rId6"/>
+    <sheet name="ignoreNull" sheetId="4" r:id="rId7"/>
+    <sheet name="ignoreBlankMap" sheetId="5" r:id="rId8"/>
+    <sheet name="ignoreBlankListTrue" sheetId="6" r:id="rId9"/>
+    <sheet name="ignoreBlankListFalse" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="78">
   <si>
     <t>noOptionTable#stringCellType</t>
     <phoneticPr fontId="1"/>
@@ -65,46 +79,6 @@
   </si>
   <si>
     <t>noOptionTable#defaultCellType</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>optionTable#~</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>optionTable#defaultCellType</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>?type=string</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>optionTable#stringCellType</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>?type=string</t>
-    </r>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -142,12 +116,445 @@
     </r>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>ignores#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ignores#id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ignoreBlankMap#id</t>
+  </si>
+  <si>
+    <t>ignoreBlankMap#~</t>
+  </si>
+  <si>
+    <t>bbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ignoreBlankListTrue#id</t>
+  </si>
+  <si>
+    <t>ignoreBlankListTrue#list[0]</t>
+  </si>
+  <si>
+    <t>ignoreBlankListTrue#list[1]</t>
+  </si>
+  <si>
+    <t>ignoreBlankListFalse#list[0]</t>
+  </si>
+  <si>
+    <t>ignoreBlankListFalse#list[1]</t>
+  </si>
+  <si>
+    <t>ignoreBlankListFalse#id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>ignores#ignoreNullFalse</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?ignoreNull=false</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>ignores#ignoredNullTrue</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?ignoreNull=true</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>ignoreBlankMap#ignoreBlankMapTrue.field</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?ignoreBlankMap=true</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>ignoreBlankMap#ignoreBlankMapFalse.field</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?ignoreBlankMap=false</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>ignoreBlankListTrue</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?ignoreBlankList=true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#~</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>ignoreBlankListFalse</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?ignoreBlankList=false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#~</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>toMapExample1.aaa, toMapExample1.bbb, toMapExample1.ccc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>toMapExample1.bbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>toMapExample1.ccc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>toMapExample1.aaa, toMapExample2.list#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Hello toMapExample1.bbb</t>
+  </si>
+  <si>
+    <t>Hello toMapExample1.ccc</t>
+  </si>
+  <si>
+    <t>Hello toMapExample1.aaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>toMapExample2.list#field1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?toMap=key</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>toMapExample2.list#field2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?toMap=value</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eee</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>bigdecimal</t>
+  </si>
+  <si>
+    <t>biginteger</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>localdatetime</t>
+  </si>
+  <si>
+    <t>localdate</t>
+  </si>
+  <si>
+    <t>localtime</t>
+  </si>
+  <si>
+    <t>fieldTypeExample#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Hello fieldType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>syntaxSugar#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>syntaxSugar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?fieldType</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>syntaxSugar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?ignoreNullBlank</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>syntaxSugar#id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>syntaxSugar#name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>syntaxSugar#dateOfBirth</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Aaa Aaaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bbb Bbbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ccc Cccc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ddd Dddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Eee Eeee</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>localdate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>readAs#defType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>readAs#defWithOption</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?readAs=text</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>readAs#strWithOption</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?readAs=text</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>readAs#strType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>readAs#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +582,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -267,7 +683,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -295,12 +711,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -615,14 +1063,14 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -633,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
@@ -641,7 +1089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -652,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -660,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -668,7 +1116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -683,72 +1131,180 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB07F82-A207-4CDA-8369-DD4798892B49}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="43.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="0.69921875" customWidth="1"/>
+    <col min="3" max="3" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="4.8" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13048F5B-FF4A-4333-83EC-A9E9FE2AB59B}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5">
+        <v>77</v>
+      </c>
+      <c r="B3" s="12">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="1">
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="3">
+      <c r="D5" s="14">
+        <v>2</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="16">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="16">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -763,123 +1319,123 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE576B48-1069-4FF4-9690-068944F0194F}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" s="1">
         <v>18</v>
       </c>
@@ -889,4 +1445,946 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B22935-1D70-417D-A4C5-EC4B351DAF54}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="37.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="0.8984375" customWidth="1"/>
+    <col min="3" max="3" width="57.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0.8984375" customWidth="1"/>
+    <col min="5" max="5" width="35.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"Hello "&amp;E3</f>
+        <v>Hello aaa</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"Hello "&amp;E4</f>
+        <v>Hello bbb</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"Hello "&amp;E5</f>
+        <v>Hello ccc</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F7" si="0">"Hello "&amp;E6</f>
+        <v>Hello ddd</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>Hello eee</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838F75B9-2F42-4701-8D73-37B59D9B2D65}">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="0.69921875" customWidth="1"/>
+    <col min="4" max="4" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="3.6" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="str">
+        <f>"fieldTypeExample#v"&amp;ROW()-2&amp;"?fieldType="&amp;B3</f>
+        <v>fieldTypeExample#v1?fieldType=string</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3">
+        <v>123</v>
+      </c>
+      <c r="F3">
+        <v>0.123456789</v>
+      </c>
+      <c r="G3">
+        <v>99999999999</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J3" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A17" si="0">"fieldTypeExample#v"&amp;ROW()-2&amp;"?fieldType="&amp;B4</f>
+        <v>fieldTypeExample#v2?fieldType=int</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>123</v>
+      </c>
+      <c r="F4">
+        <v>0.123456789</v>
+      </c>
+      <c r="G4">
+        <v>99999999999</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J4" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v3?fieldType=long</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <v>123</v>
+      </c>
+      <c r="F5">
+        <v>0.123456789</v>
+      </c>
+      <c r="G5">
+        <v>99999999999</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J5" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v4?fieldType=char</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6">
+        <v>123</v>
+      </c>
+      <c r="F6">
+        <v>0.123456789</v>
+      </c>
+      <c r="G6">
+        <v>99999999999</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J6" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v5?fieldType=boolean</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7">
+        <v>123</v>
+      </c>
+      <c r="F7">
+        <v>0.123456789</v>
+      </c>
+      <c r="G7">
+        <v>99999999999</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J7" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v6?fieldType=byte</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8">
+        <v>123</v>
+      </c>
+      <c r="F8">
+        <v>0.123456789</v>
+      </c>
+      <c r="G8">
+        <v>99999999999</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J8" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v7?fieldType=short</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9">
+        <v>123</v>
+      </c>
+      <c r="F9">
+        <v>0.123456789</v>
+      </c>
+      <c r="G9">
+        <v>99999999999</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J9" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v8?fieldType=float</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10">
+        <v>123</v>
+      </c>
+      <c r="F10">
+        <v>0.123456789</v>
+      </c>
+      <c r="G10">
+        <v>99999999999</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J10" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v9?fieldType=double</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11">
+        <v>123</v>
+      </c>
+      <c r="F11">
+        <v>0.123456789</v>
+      </c>
+      <c r="G11">
+        <v>99999999999</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J11" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v10?fieldType=bigdecimal</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>123</v>
+      </c>
+      <c r="F12">
+        <v>0.123456789</v>
+      </c>
+      <c r="G12">
+        <v>99999999999</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J12" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v11?fieldType=biginteger</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13">
+        <v>123</v>
+      </c>
+      <c r="F13">
+        <v>0.123456789</v>
+      </c>
+      <c r="G13">
+        <v>99999999999</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J13" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v12?fieldType=date</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14">
+        <v>123</v>
+      </c>
+      <c r="F14">
+        <v>0.123456789</v>
+      </c>
+      <c r="G14">
+        <v>99999999999</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J14" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v13?fieldType=localdatetime</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15">
+        <v>123</v>
+      </c>
+      <c r="F15">
+        <v>0.123456789</v>
+      </c>
+      <c r="G15">
+        <v>99999999999</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J15" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v14?fieldType=localdate</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16">
+        <v>123</v>
+      </c>
+      <c r="F16">
+        <v>0.123456789</v>
+      </c>
+      <c r="G16">
+        <v>99999999999</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J16" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldTypeExample#v15?fieldType=localtime</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <v>123</v>
+      </c>
+      <c r="F17">
+        <v>0.123456789</v>
+      </c>
+      <c r="G17">
+        <v>99999999999</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>43466</v>
+      </c>
+      <c r="J17" s="10">
+        <v>43466.524259259262</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C54912B-BF87-423E-A0B3-0BBF7AA74CE8}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="0.5" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="3.6" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="3.6" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="9">
+        <v>32874</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="9">
+        <v>29221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="9">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E142DF-9A02-4391-8A79-6AB89A6F91A4}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="0.8984375" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" customWidth="1"/>
+    <col min="4" max="4" width="38.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="3.6" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C0D3B8-B8B2-4D3A-A928-A5A9AAEA3B37}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.19921875" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="3.6" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F30EFA1-B190-4560-AC1E-9BBE1B4C9B40}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="0.5" customWidth="1"/>
+    <col min="3" max="3" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="2.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>